<commit_message>
Updating the backend and adding new functions
</commit_message>
<xml_diff>
--- a/backend/exports/Bewertungsdaten.xlsx
+++ b/backend/exports/Bewertungsdaten.xlsx
@@ -4,8 +4,9 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="Students" sheetId="1" r:id="rId1"/>
-    <sheet name="Exercises" sheetId="2" r:id="rId2"/>
-    <sheet name="Thresholds" sheetId="3" r:id="rId3"/>
+    <sheet name="Aufgaben" sheetId="2" r:id="rId2"/>
+    <sheet name="Grenzwerte" sheetId="3" r:id="rId3"/>
+    <sheet name="Module Info" sheetId="4" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -415,16 +416,16 @@
         <v>Vorname</v>
       </c>
       <c r="D1" t="str">
-        <v>AUF1</v>
+        <v>Auf 1</v>
       </c>
       <c r="E1" t="str">
-        <v>AUF2</v>
+        <v>Auf 2</v>
       </c>
       <c r="F1" t="str">
-        <v>AUF3</v>
+        <v>Auf 3</v>
       </c>
       <c r="G1" t="str">
-        <v>AUF4</v>
+        <v>Auf 4</v>
       </c>
       <c r="H1" t="str">
         <v>Total</v>
@@ -589,22 +590,22 @@
         <v>Jonas</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7" t="str">
-        <v>ne</v>
-      </c>
-      <c r="I7" t="str">
-        <v/>
+        <v>28.5</v>
+      </c>
+      <c r="H7">
+        <v>59.5</v>
+      </c>
+      <c r="I7">
+        <v>83</v>
       </c>
     </row>
     <row r="8">
@@ -621,19 +622,19 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8" t="str">
-        <v>ne</v>
-      </c>
-      <c r="I8" t="str">
-        <v/>
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>14.5</v>
+      </c>
+      <c r="I8">
+        <v>21</v>
       </c>
     </row>
     <row r="9">
@@ -646,23 +647,11 @@
       <c r="C9" t="str">
         <v>Liam</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
       <c r="H9" t="str">
-        <v>ne</v>
+        <v xml:space="preserve">                   ne</v>
       </c>
       <c r="I9" t="str">
-        <v/>
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="10">
@@ -675,23 +664,11 @@
       <c r="C10" t="str">
         <v>Noah</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
       <c r="H10" t="str">
-        <v>ne</v>
+        <v xml:space="preserve">                   ne</v>
       </c>
       <c r="I10" t="str">
-        <v/>
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="11">
@@ -708,7 +685,7 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -716,11 +693,11 @@
       <c r="G11">
         <v>0</v>
       </c>
-      <c r="H11" t="str">
-        <v>ne</v>
-      </c>
-      <c r="I11" t="str">
-        <v/>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -734,22 +711,22 @@
         <v>Finn</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12" t="str">
-        <v>ne</v>
-      </c>
-      <c r="I12" t="str">
-        <v/>
+        <v>17</v>
+      </c>
+      <c r="H12">
+        <v>51</v>
+      </c>
+      <c r="I12">
+        <v>75</v>
       </c>
     </row>
     <row r="13">
@@ -763,22 +740,22 @@
         <v>Julian</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>10.5</v>
       </c>
       <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13" t="str">
-        <v>ne</v>
-      </c>
-      <c r="I13" t="str">
-        <v/>
+        <v>5</v>
+      </c>
+      <c r="H13">
+        <v>29.5</v>
+      </c>
+      <c r="I13">
+        <v>43</v>
       </c>
     </row>
     <row r="14">
@@ -792,22 +769,22 @@
         <v>Tim</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14" t="str">
-        <v>ne</v>
-      </c>
-      <c r="I14" t="str">
-        <v/>
+        <v>24</v>
+      </c>
+      <c r="H14">
+        <v>62</v>
+      </c>
+      <c r="I14">
+        <v>87</v>
       </c>
     </row>
     <row r="15">
@@ -821,22 +798,22 @@
         <v>Tom</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15" t="str">
-        <v>ne</v>
-      </c>
-      <c r="I15" t="str">
-        <v/>
+        <v>5</v>
+      </c>
+      <c r="H15">
+        <v>35</v>
+      </c>
+      <c r="I15">
+        <v>51</v>
       </c>
     </row>
     <row r="16">
@@ -850,22 +827,22 @@
         <v>Milan</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16" t="str">
-        <v>ne</v>
-      </c>
-      <c r="I16" t="str">
-        <v/>
+        <v>3</v>
+      </c>
+      <c r="H16">
+        <v>25</v>
+      </c>
+      <c r="I16">
+        <v>37</v>
       </c>
     </row>
     <row r="17">
@@ -879,22 +856,22 @@
         <v>David</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17" t="str">
-        <v>ne</v>
-      </c>
-      <c r="I17" t="str">
-        <v/>
+        <v>11</v>
+      </c>
+      <c r="H17">
+        <v>35</v>
+      </c>
+      <c r="I17">
+        <v>51</v>
       </c>
     </row>
     <row r="18">
@@ -908,22 +885,22 @@
         <v>Emil</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18" t="str">
-        <v>ne</v>
-      </c>
-      <c r="I18" t="str">
-        <v/>
+        <v>9</v>
+      </c>
+      <c r="H18">
+        <v>37</v>
+      </c>
+      <c r="I18">
+        <v>54</v>
       </c>
     </row>
     <row r="19">
@@ -937,22 +914,22 @@
         <v>Ben</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19" t="str">
-        <v>ne</v>
-      </c>
-      <c r="I19" t="str">
-        <v/>
+        <v>11</v>
+      </c>
+      <c r="H19">
+        <v>59</v>
+      </c>
+      <c r="I19">
+        <v>82</v>
       </c>
     </row>
     <row r="20">
@@ -966,22 +943,22 @@
         <v>Mia</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20" t="str">
-        <v>ne</v>
-      </c>
-      <c r="I20" t="str">
-        <v/>
+        <v>7</v>
+      </c>
+      <c r="H20">
+        <v>31</v>
+      </c>
+      <c r="I20">
+        <v>46</v>
       </c>
     </row>
     <row r="21">
@@ -995,22 +972,22 @@
         <v>Emma</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21" t="str">
-        <v>ne</v>
-      </c>
-      <c r="I21" t="str">
-        <v/>
+        <v>29</v>
+      </c>
+      <c r="H21">
+        <v>62</v>
+      </c>
+      <c r="I21">
+        <v>87</v>
       </c>
     </row>
     <row r="22">
@@ -1027,19 +1004,19 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22" t="str">
-        <v>ne</v>
-      </c>
-      <c r="I22" t="str">
-        <v/>
+        <v>2</v>
+      </c>
+      <c r="H22">
+        <v>19</v>
+      </c>
+      <c r="I22">
+        <v>28</v>
       </c>
     </row>
     <row r="23">
@@ -1053,22 +1030,22 @@
         <v>Hannah</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23" t="str">
-        <v>ne</v>
-      </c>
-      <c r="I23" t="str">
-        <v/>
+        <v>15.5</v>
+      </c>
+      <c r="H23">
+        <v>56.5</v>
+      </c>
+      <c r="I23">
+        <v>79</v>
       </c>
     </row>
     <row r="24">
@@ -1082,22 +1059,22 @@
         <v>Lea</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24" t="str">
-        <v>ne</v>
-      </c>
-      <c r="I24" t="str">
-        <v/>
+        <v>17</v>
+      </c>
+      <c r="H24">
+        <v>46</v>
+      </c>
+      <c r="I24">
+        <v>68</v>
       </c>
     </row>
     <row r="25">
@@ -1110,23 +1087,11 @@
       <c r="C25" t="str">
         <v>Anna</v>
       </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
       <c r="H25" t="str">
-        <v>ne</v>
+        <v xml:space="preserve">                   ne</v>
       </c>
       <c r="I25" t="str">
-        <v/>
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="26">
@@ -1140,22 +1105,22 @@
         <v>Marie</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="G26">
         <v>0</v>
       </c>
-      <c r="H26" t="str">
-        <v>ne</v>
-      </c>
-      <c r="I26" t="str">
-        <v/>
+      <c r="H26">
+        <v>4.5</v>
+      </c>
+      <c r="I26">
+        <v>7</v>
       </c>
     </row>
     <row r="27">
@@ -1168,23 +1133,11 @@
       <c r="C27" t="str">
         <v>Lina</v>
       </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
       <c r="H27" t="str">
-        <v>ne</v>
+        <v xml:space="preserve">                   ne</v>
       </c>
       <c r="I27" t="str">
-        <v/>
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="28">
@@ -1210,10 +1163,10 @@
         <v>0</v>
       </c>
       <c r="H28" t="str">
-        <v>ne</v>
+        <v xml:space="preserve">                   ne</v>
       </c>
       <c r="I28" t="str">
-        <v/>
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="29">
@@ -1239,10 +1192,10 @@
         <v>0</v>
       </c>
       <c r="H29" t="str">
-        <v>ne</v>
+        <v xml:space="preserve">                   ne</v>
       </c>
       <c r="I29" t="str">
-        <v/>
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="30">
@@ -1268,10 +1221,10 @@
         <v>0</v>
       </c>
       <c r="H30" t="str">
-        <v>ne</v>
+        <v xml:space="preserve">                   ne</v>
       </c>
       <c r="I30" t="str">
-        <v/>
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="31">
@@ -1297,10 +1250,10 @@
         <v>0</v>
       </c>
       <c r="H31" t="str">
-        <v>ne</v>
+        <v xml:space="preserve">                   ne</v>
       </c>
       <c r="I31" t="str">
-        <v/>
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="32">
@@ -1326,10 +1279,10 @@
         <v>0</v>
       </c>
       <c r="H32" t="str">
-        <v>ne</v>
+        <v xml:space="preserve">                   ne</v>
       </c>
       <c r="I32" t="str">
-        <v/>
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="33">
@@ -1355,10 +1308,10 @@
         <v>0</v>
       </c>
       <c r="H33" t="str">
-        <v>ne</v>
+        <v xml:space="preserve">                   ne</v>
       </c>
       <c r="I33" t="str">
-        <v/>
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="34">
@@ -1384,10 +1337,10 @@
         <v>0</v>
       </c>
       <c r="H34" t="str">
-        <v>ne</v>
+        <v xml:space="preserve">                   ne</v>
       </c>
       <c r="I34" t="str">
-        <v/>
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="35">
@@ -1413,10 +1366,10 @@
         <v>0</v>
       </c>
       <c r="H35" t="str">
-        <v>ne</v>
+        <v xml:space="preserve">                   ne</v>
       </c>
       <c r="I35" t="str">
-        <v/>
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="36">
@@ -1442,10 +1395,10 @@
         <v>0</v>
       </c>
       <c r="H36" t="str">
-        <v>ne</v>
+        <v xml:space="preserve">                   ne</v>
       </c>
       <c r="I36" t="str">
-        <v/>
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="37">
@@ -1471,10 +1424,10 @@
         <v>0</v>
       </c>
       <c r="H37" t="str">
-        <v>ne</v>
+        <v xml:space="preserve">                   ne</v>
       </c>
       <c r="I37" t="str">
-        <v/>
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="38">
@@ -1500,10 +1453,10 @@
         <v>0</v>
       </c>
       <c r="H38" t="str">
-        <v>ne</v>
+        <v xml:space="preserve">                   ne</v>
       </c>
       <c r="I38" t="str">
-        <v/>
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="39">
@@ -1529,10 +1482,10 @@
         <v>0</v>
       </c>
       <c r="H39" t="str">
-        <v>ne</v>
+        <v xml:space="preserve">                   ne</v>
       </c>
       <c r="I39" t="str">
-        <v/>
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="40">
@@ -1558,10 +1511,10 @@
         <v>0</v>
       </c>
       <c r="H40" t="str">
-        <v>ne</v>
+        <v xml:space="preserve">                   ne</v>
       </c>
       <c r="I40" t="str">
-        <v/>
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="41">
@@ -1587,10 +1540,10 @@
         <v>0</v>
       </c>
       <c r="H41" t="str">
-        <v>ne</v>
+        <v xml:space="preserve">                   ne</v>
       </c>
       <c r="I41" t="str">
-        <v/>
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="42">
@@ -1616,10 +1569,10 @@
         <v>0</v>
       </c>
       <c r="H42" t="str">
-        <v>ne</v>
+        <v xml:space="preserve">                   ne</v>
       </c>
       <c r="I42" t="str">
-        <v/>
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="43">
@@ -1645,10 +1598,10 @@
         <v>0</v>
       </c>
       <c r="H43" t="str">
-        <v>ne</v>
+        <v xml:space="preserve">                   ne</v>
       </c>
       <c r="I43" t="str">
-        <v/>
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="44">
@@ -1674,10 +1627,10 @@
         <v>0</v>
       </c>
       <c r="H44" t="str">
-        <v>ne</v>
+        <v xml:space="preserve">                   ne</v>
       </c>
       <c r="I44" t="str">
-        <v/>
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="45">
@@ -1703,10 +1656,10 @@
         <v>0</v>
       </c>
       <c r="H45" t="str">
-        <v>ne</v>
+        <v xml:space="preserve">                   ne</v>
       </c>
       <c r="I45" t="str">
-        <v/>
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="46">
@@ -1732,10 +1685,10 @@
         <v>0</v>
       </c>
       <c r="H46" t="str">
-        <v>ne</v>
+        <v xml:space="preserve">                   ne</v>
       </c>
       <c r="I46" t="str">
-        <v/>
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="47">
@@ -1761,10 +1714,10 @@
         <v>0</v>
       </c>
       <c r="H47" t="str">
-        <v>ne</v>
+        <v xml:space="preserve">                   ne</v>
       </c>
       <c r="I47" t="str">
-        <v/>
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="48">
@@ -1778,22 +1731,22 @@
         <v>Fatma</v>
       </c>
       <c r="D48">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E48">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="F48">
-        <v>15.5</v>
+        <v>0</v>
       </c>
       <c r="G48">
-        <v>26</v>
-      </c>
-      <c r="H48">
-        <v>65.5</v>
-      </c>
-      <c r="I48">
-        <v>92</v>
+        <v>0</v>
+      </c>
+      <c r="H48" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="I48" t="str">
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="49">
@@ -1807,22 +1760,22 @@
         <v>Aylin</v>
       </c>
       <c r="D49">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E49">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F49">
-        <v>8.5</v>
+        <v>0</v>
       </c>
       <c r="G49">
-        <v>4</v>
-      </c>
-      <c r="H49">
-        <v>23.5</v>
-      </c>
-      <c r="I49">
-        <v>35</v>
+        <v>0</v>
+      </c>
+      <c r="H49" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="I49" t="str">
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="50">
@@ -1836,22 +1789,22 @@
         <v>Leyla</v>
       </c>
       <c r="D50">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E50">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F50">
-        <v>9.5</v>
+        <v>0</v>
       </c>
       <c r="G50">
-        <v>8</v>
-      </c>
-      <c r="H50">
-        <v>36.5</v>
-      </c>
-      <c r="I50">
-        <v>54</v>
+        <v>0</v>
+      </c>
+      <c r="H50" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="I50" t="str">
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="51">
@@ -1877,10 +1830,10 @@
         <v>0</v>
       </c>
       <c r="H51" t="str">
-        <v>ne</v>
+        <v xml:space="preserve">                   ne</v>
       </c>
       <c r="I51" t="str">
-        <v/>
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
   </sheetData>
@@ -1902,12 +1855,12 @@
         <v>Aufgaben</v>
       </c>
       <c r="B1" t="str">
-        <v>Gewicht</v>
+        <v>Anzahl_Punktzahl</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>AUF1</v>
+        <v>Auf 1</v>
       </c>
       <c r="B2">
         <v>9</v>
@@ -1915,23 +1868,23 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>AUF2</v>
+        <v>Auf 2</v>
       </c>
       <c r="B3">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>AUF3</v>
+        <v>Auf 3</v>
       </c>
       <c r="B4">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>AUF4</v>
+        <v>Auf 4</v>
       </c>
       <c r="B5">
         <v>32</v>
@@ -1946,7 +1899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1995,9 +1948,86 @@
         <v>1.3</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5">
+        <v>77</v>
+      </c>
+      <c r="B5" t="str">
+        <v>100%</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C5"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Module Eigenschaft</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Module Information</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Module Title</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Webbasierte Systeme</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Module Number</v>
+      </c>
+      <c r="B3" t="str">
+        <v>CS1024</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Prüfungsdatum</v>
+      </c>
+      <c r="B4" t="str">
+        <v>2025-02-27</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Prüfer</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Herr Müller</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Exportdatum</v>
+      </c>
+      <c r="B6" t="str">
+        <v>24.2.2025</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:B6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modification of the backend structure and frontend design
</commit_message>
<xml_diff>
--- a/backend/exports/Bewertungsdaten.xlsx
+++ b/backend/exports/Bewertungsdaten.xlsx
@@ -400,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -416,21 +416,15 @@
         <v>Vorname</v>
       </c>
       <c r="D1" t="str">
-        <v>Auf 1</v>
+        <v>dfe</v>
       </c>
       <c r="E1" t="str">
-        <v>Auf 2</v>
+        <v>ewwr</v>
       </c>
       <c r="F1" t="str">
-        <v>Auf 3</v>
+        <v>Gesamt</v>
       </c>
       <c r="G1" t="str">
-        <v>Auf 4</v>
-      </c>
-      <c r="H1" t="str">
-        <v>Total</v>
-      </c>
-      <c r="I1" t="str">
         <v>Bewertung</v>
       </c>
     </row>
@@ -445,22 +439,16 @@
         <v>Max</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="E2">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="F2">
-        <v>12.5</v>
+        <v>48</v>
       </c>
       <c r="G2">
-        <v>11</v>
-      </c>
-      <c r="H2">
-        <v>37.5</v>
-      </c>
-      <c r="I2">
-        <v>55</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3">
@@ -474,22 +462,16 @@
         <v>Paul</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="E3">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="F3">
-        <v>12.5</v>
+        <v>66</v>
       </c>
       <c r="G3">
-        <v>17.5</v>
-      </c>
-      <c r="H3">
-        <v>57</v>
-      </c>
-      <c r="I3">
-        <v>80</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4">
@@ -503,22 +485,16 @@
         <v>Alexander</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="E4">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="F4">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>22</v>
-      </c>
-      <c r="I4">
-        <v>32</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5">
@@ -532,22 +508,16 @@
         <v>Lukas</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>3.5</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>7.5</v>
-      </c>
-      <c r="I5">
-        <v>11</v>
+        <v>0</v>
+      </c>
+      <c r="F5" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G5" t="str">
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="6">
@@ -561,22 +531,16 @@
         <v>Leon</v>
       </c>
       <c r="D6">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>16</v>
-      </c>
-      <c r="F6">
-        <v>17</v>
-      </c>
-      <c r="G6">
-        <v>24.5</v>
-      </c>
-      <c r="H6">
-        <v>65.5</v>
-      </c>
-      <c r="I6">
-        <v>92</v>
+        <v>0</v>
+      </c>
+      <c r="F6" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G6" t="str">
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="7">
@@ -590,22 +554,16 @@
         <v>Jonas</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>19</v>
-      </c>
-      <c r="F7">
-        <v>8</v>
-      </c>
-      <c r="G7">
-        <v>28.5</v>
-      </c>
-      <c r="H7">
-        <v>59.5</v>
-      </c>
-      <c r="I7">
-        <v>83</v>
+        <v>0</v>
+      </c>
+      <c r="F7" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G7" t="str">
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="8">
@@ -622,19 +580,13 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>6</v>
-      </c>
-      <c r="F8">
-        <v>7.5</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>14.5</v>
-      </c>
-      <c r="I8">
-        <v>21</v>
+        <v>0</v>
+      </c>
+      <c r="F8" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G8" t="str">
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="9">
@@ -647,10 +599,16 @@
       <c r="C9" t="str">
         <v>Liam</v>
       </c>
-      <c r="H9" t="str">
-        <v xml:space="preserve">                   ne</v>
-      </c>
-      <c r="I9" t="str">
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G9" t="str">
         <v xml:space="preserve">                   ne</v>
       </c>
     </row>
@@ -664,10 +622,16 @@
       <c r="C10" t="str">
         <v>Noah</v>
       </c>
-      <c r="H10" t="str">
-        <v xml:space="preserve">                   ne</v>
-      </c>
-      <c r="I10" t="str">
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G10" t="str">
         <v xml:space="preserve">                   ne</v>
       </c>
     </row>
@@ -685,19 +649,13 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F11" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G11" t="str">
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="12">
@@ -711,22 +669,16 @@
         <v>Finn</v>
       </c>
       <c r="D12">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>11</v>
-      </c>
-      <c r="F12">
-        <v>16</v>
-      </c>
-      <c r="G12">
-        <v>17</v>
-      </c>
-      <c r="H12">
-        <v>51</v>
-      </c>
-      <c r="I12">
-        <v>75</v>
+        <v>0</v>
+      </c>
+      <c r="F12" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G12" t="str">
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="13">
@@ -740,22 +692,16 @@
         <v>Julian</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>12</v>
-      </c>
-      <c r="F13">
-        <v>10.5</v>
-      </c>
-      <c r="G13">
-        <v>5</v>
-      </c>
-      <c r="H13">
-        <v>29.5</v>
-      </c>
-      <c r="I13">
-        <v>43</v>
+        <v>0</v>
+      </c>
+      <c r="F13" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G13" t="str">
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="14">
@@ -769,22 +715,16 @@
         <v>Tim</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>21</v>
-      </c>
-      <c r="F14">
-        <v>14</v>
-      </c>
-      <c r="G14">
-        <v>24</v>
-      </c>
-      <c r="H14">
-        <v>62</v>
-      </c>
-      <c r="I14">
-        <v>87</v>
+        <v>0</v>
+      </c>
+      <c r="F14" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G14" t="str">
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="15">
@@ -798,22 +738,16 @@
         <v>Tom</v>
       </c>
       <c r="D15">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>9</v>
-      </c>
-      <c r="F15">
-        <v>15</v>
-      </c>
-      <c r="G15">
-        <v>5</v>
-      </c>
-      <c r="H15">
-        <v>35</v>
-      </c>
-      <c r="I15">
-        <v>51</v>
+        <v>0</v>
+      </c>
+      <c r="F15" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G15" t="str">
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="16">
@@ -827,22 +761,16 @@
         <v>Milan</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>8</v>
-      </c>
-      <c r="F16">
-        <v>11</v>
-      </c>
-      <c r="G16">
-        <v>3</v>
-      </c>
-      <c r="H16">
-        <v>25</v>
-      </c>
-      <c r="I16">
-        <v>37</v>
+        <v>0</v>
+      </c>
+      <c r="F16" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G16" t="str">
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="17">
@@ -856,22 +784,16 @@
         <v>David</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>6</v>
-      </c>
-      <c r="F17">
-        <v>15</v>
-      </c>
-      <c r="G17">
-        <v>11</v>
-      </c>
-      <c r="H17">
-        <v>35</v>
-      </c>
-      <c r="I17">
-        <v>51</v>
+        <v>0</v>
+      </c>
+      <c r="F17" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G17" t="str">
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="18">
@@ -885,22 +807,16 @@
         <v>Emil</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>14</v>
-      </c>
-      <c r="F18">
-        <v>13</v>
-      </c>
-      <c r="G18">
-        <v>9</v>
-      </c>
-      <c r="H18">
-        <v>37</v>
-      </c>
-      <c r="I18">
-        <v>54</v>
+        <v>0</v>
+      </c>
+      <c r="F18" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G18" t="str">
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="19">
@@ -914,22 +830,16 @@
         <v>Ben</v>
       </c>
       <c r="D19">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>22</v>
-      </c>
-      <c r="F19">
-        <v>17</v>
-      </c>
-      <c r="G19">
-        <v>11</v>
-      </c>
-      <c r="H19">
-        <v>59</v>
-      </c>
-      <c r="I19">
-        <v>82</v>
+        <v>0</v>
+      </c>
+      <c r="F19" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G19" t="str">
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="20">
@@ -943,22 +853,16 @@
         <v>Mia</v>
       </c>
       <c r="D20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>11</v>
-      </c>
-      <c r="F20">
-        <v>11</v>
-      </c>
-      <c r="G20">
-        <v>7</v>
-      </c>
-      <c r="H20">
-        <v>31</v>
-      </c>
-      <c r="I20">
-        <v>46</v>
+        <v>0</v>
+      </c>
+      <c r="F20" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G20" t="str">
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="21">
@@ -972,22 +876,16 @@
         <v>Emma</v>
       </c>
       <c r="D21">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>15</v>
-      </c>
-      <c r="F21">
-        <v>15</v>
-      </c>
-      <c r="G21">
-        <v>29</v>
-      </c>
-      <c r="H21">
-        <v>62</v>
-      </c>
-      <c r="I21">
-        <v>87</v>
+        <v>0</v>
+      </c>
+      <c r="F21" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G21" t="str">
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="22">
@@ -1004,19 +902,13 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>5</v>
-      </c>
-      <c r="F22">
-        <v>12</v>
-      </c>
-      <c r="G22">
-        <v>2</v>
-      </c>
-      <c r="H22">
-        <v>19</v>
-      </c>
-      <c r="I22">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="F22" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G22" t="str">
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="23">
@@ -1030,22 +922,16 @@
         <v>Hannah</v>
       </c>
       <c r="D23">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E23">
-        <v>19</v>
-      </c>
-      <c r="F23">
-        <v>16</v>
-      </c>
-      <c r="G23">
-        <v>15.5</v>
-      </c>
-      <c r="H23">
-        <v>56.5</v>
-      </c>
-      <c r="I23">
-        <v>79</v>
+        <v>0</v>
+      </c>
+      <c r="F23" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G23" t="str">
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="24">
@@ -1059,22 +945,16 @@
         <v>Lea</v>
       </c>
       <c r="D24">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>12</v>
-      </c>
-      <c r="F24">
-        <v>13</v>
-      </c>
-      <c r="G24">
-        <v>17</v>
-      </c>
-      <c r="H24">
-        <v>46</v>
-      </c>
-      <c r="I24">
-        <v>68</v>
+        <v>0</v>
+      </c>
+      <c r="F24" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G24" t="str">
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="25">
@@ -1087,10 +967,16 @@
       <c r="C25" t="str">
         <v>Anna</v>
       </c>
-      <c r="H25" t="str">
-        <v xml:space="preserve">                   ne</v>
-      </c>
-      <c r="I25" t="str">
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G25" t="str">
         <v xml:space="preserve">                   ne</v>
       </c>
     </row>
@@ -1105,22 +991,16 @@
         <v>Marie</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>2.5</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26">
-        <v>4.5</v>
-      </c>
-      <c r="I26">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="F26" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G26" t="str">
+        <v xml:space="preserve">                   ne</v>
       </c>
     </row>
     <row r="27">
@@ -1133,10 +1013,16 @@
       <c r="C27" t="str">
         <v>Lina</v>
       </c>
-      <c r="H27" t="str">
-        <v xml:space="preserve">                   ne</v>
-      </c>
-      <c r="I27" t="str">
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G27" t="str">
         <v xml:space="preserve">                   ne</v>
       </c>
     </row>
@@ -1156,16 +1042,10 @@
       <c r="E28">
         <v>0</v>
       </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28" t="str">
-        <v xml:space="preserve">                   ne</v>
-      </c>
-      <c r="I28" t="str">
+      <c r="F28" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G28" t="str">
         <v xml:space="preserve">                   ne</v>
       </c>
     </row>
@@ -1185,16 +1065,10 @@
       <c r="E29">
         <v>0</v>
       </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29" t="str">
-        <v xml:space="preserve">                   ne</v>
-      </c>
-      <c r="I29" t="str">
+      <c r="F29" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G29" t="str">
         <v xml:space="preserve">                   ne</v>
       </c>
     </row>
@@ -1214,16 +1088,10 @@
       <c r="E30">
         <v>0</v>
       </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30" t="str">
-        <v xml:space="preserve">                   ne</v>
-      </c>
-      <c r="I30" t="str">
+      <c r="F30" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G30" t="str">
         <v xml:space="preserve">                   ne</v>
       </c>
     </row>
@@ -1243,16 +1111,10 @@
       <c r="E31">
         <v>0</v>
       </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-      <c r="H31" t="str">
-        <v xml:space="preserve">                   ne</v>
-      </c>
-      <c r="I31" t="str">
+      <c r="F31" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G31" t="str">
         <v xml:space="preserve">                   ne</v>
       </c>
     </row>
@@ -1272,16 +1134,10 @@
       <c r="E32">
         <v>0</v>
       </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32" t="str">
-        <v xml:space="preserve">                   ne</v>
-      </c>
-      <c r="I32" t="str">
+      <c r="F32" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G32" t="str">
         <v xml:space="preserve">                   ne</v>
       </c>
     </row>
@@ -1301,16 +1157,10 @@
       <c r="E33">
         <v>0</v>
       </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-      <c r="H33" t="str">
-        <v xml:space="preserve">                   ne</v>
-      </c>
-      <c r="I33" t="str">
+      <c r="F33" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G33" t="str">
         <v xml:space="preserve">                   ne</v>
       </c>
     </row>
@@ -1330,16 +1180,10 @@
       <c r="E34">
         <v>0</v>
       </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="H34" t="str">
-        <v xml:space="preserve">                   ne</v>
-      </c>
-      <c r="I34" t="str">
+      <c r="F34" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G34" t="str">
         <v xml:space="preserve">                   ne</v>
       </c>
     </row>
@@ -1359,16 +1203,10 @@
       <c r="E35">
         <v>0</v>
       </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-      <c r="H35" t="str">
-        <v xml:space="preserve">                   ne</v>
-      </c>
-      <c r="I35" t="str">
+      <c r="F35" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G35" t="str">
         <v xml:space="preserve">                   ne</v>
       </c>
     </row>
@@ -1388,16 +1226,10 @@
       <c r="E36">
         <v>0</v>
       </c>
-      <c r="F36">
-        <v>0</v>
-      </c>
-      <c r="G36">
-        <v>0</v>
-      </c>
-      <c r="H36" t="str">
-        <v xml:space="preserve">                   ne</v>
-      </c>
-      <c r="I36" t="str">
+      <c r="F36" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G36" t="str">
         <v xml:space="preserve">                   ne</v>
       </c>
     </row>
@@ -1417,16 +1249,10 @@
       <c r="E37">
         <v>0</v>
       </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
-      <c r="H37" t="str">
-        <v xml:space="preserve">                   ne</v>
-      </c>
-      <c r="I37" t="str">
+      <c r="F37" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G37" t="str">
         <v xml:space="preserve">                   ne</v>
       </c>
     </row>
@@ -1446,16 +1272,10 @@
       <c r="E38">
         <v>0</v>
       </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
-      <c r="H38" t="str">
-        <v xml:space="preserve">                   ne</v>
-      </c>
-      <c r="I38" t="str">
+      <c r="F38" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G38" t="str">
         <v xml:space="preserve">                   ne</v>
       </c>
     </row>
@@ -1475,16 +1295,10 @@
       <c r="E39">
         <v>0</v>
       </c>
-      <c r="F39">
-        <v>0</v>
-      </c>
-      <c r="G39">
-        <v>0</v>
-      </c>
-      <c r="H39" t="str">
-        <v xml:space="preserve">                   ne</v>
-      </c>
-      <c r="I39" t="str">
+      <c r="F39" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G39" t="str">
         <v xml:space="preserve">                   ne</v>
       </c>
     </row>
@@ -1504,16 +1318,10 @@
       <c r="E40">
         <v>0</v>
       </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
-      <c r="H40" t="str">
-        <v xml:space="preserve">                   ne</v>
-      </c>
-      <c r="I40" t="str">
+      <c r="F40" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G40" t="str">
         <v xml:space="preserve">                   ne</v>
       </c>
     </row>
@@ -1533,16 +1341,10 @@
       <c r="E41">
         <v>0</v>
       </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
-      <c r="H41" t="str">
-        <v xml:space="preserve">                   ne</v>
-      </c>
-      <c r="I41" t="str">
+      <c r="F41" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G41" t="str">
         <v xml:space="preserve">                   ne</v>
       </c>
     </row>
@@ -1562,16 +1364,10 @@
       <c r="E42">
         <v>0</v>
       </c>
-      <c r="F42">
-        <v>0</v>
-      </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
-      <c r="H42" t="str">
-        <v xml:space="preserve">                   ne</v>
-      </c>
-      <c r="I42" t="str">
+      <c r="F42" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G42" t="str">
         <v xml:space="preserve">                   ne</v>
       </c>
     </row>
@@ -1591,16 +1387,10 @@
       <c r="E43">
         <v>0</v>
       </c>
-      <c r="F43">
-        <v>0</v>
-      </c>
-      <c r="G43">
-        <v>0</v>
-      </c>
-      <c r="H43" t="str">
-        <v xml:space="preserve">                   ne</v>
-      </c>
-      <c r="I43" t="str">
+      <c r="F43" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G43" t="str">
         <v xml:space="preserve">                   ne</v>
       </c>
     </row>
@@ -1620,16 +1410,10 @@
       <c r="E44">
         <v>0</v>
       </c>
-      <c r="F44">
-        <v>0</v>
-      </c>
-      <c r="G44">
-        <v>0</v>
-      </c>
-      <c r="H44" t="str">
-        <v xml:space="preserve">                   ne</v>
-      </c>
-      <c r="I44" t="str">
+      <c r="F44" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G44" t="str">
         <v xml:space="preserve">                   ne</v>
       </c>
     </row>
@@ -1649,16 +1433,10 @@
       <c r="E45">
         <v>0</v>
       </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
-      <c r="G45">
-        <v>0</v>
-      </c>
-      <c r="H45" t="str">
-        <v xml:space="preserve">                   ne</v>
-      </c>
-      <c r="I45" t="str">
+      <c r="F45" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G45" t="str">
         <v xml:space="preserve">                   ne</v>
       </c>
     </row>
@@ -1678,16 +1456,10 @@
       <c r="E46">
         <v>0</v>
       </c>
-      <c r="F46">
-        <v>0</v>
-      </c>
-      <c r="G46">
-        <v>0</v>
-      </c>
-      <c r="H46" t="str">
-        <v xml:space="preserve">                   ne</v>
-      </c>
-      <c r="I46" t="str">
+      <c r="F46" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G46" t="str">
         <v xml:space="preserve">                   ne</v>
       </c>
     </row>
@@ -1707,16 +1479,10 @@
       <c r="E47">
         <v>0</v>
       </c>
-      <c r="F47">
-        <v>0</v>
-      </c>
-      <c r="G47">
-        <v>0</v>
-      </c>
-      <c r="H47" t="str">
-        <v xml:space="preserve">                   ne</v>
-      </c>
-      <c r="I47" t="str">
+      <c r="F47" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G47" t="str">
         <v xml:space="preserve">                   ne</v>
       </c>
     </row>
@@ -1736,16 +1502,10 @@
       <c r="E48">
         <v>0</v>
       </c>
-      <c r="F48">
-        <v>0</v>
-      </c>
-      <c r="G48">
-        <v>0</v>
-      </c>
-      <c r="H48" t="str">
-        <v xml:space="preserve">                   ne</v>
-      </c>
-      <c r="I48" t="str">
+      <c r="F48" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G48" t="str">
         <v xml:space="preserve">                   ne</v>
       </c>
     </row>
@@ -1765,16 +1525,10 @@
       <c r="E49">
         <v>0</v>
       </c>
-      <c r="F49">
-        <v>0</v>
-      </c>
-      <c r="G49">
-        <v>0</v>
-      </c>
-      <c r="H49" t="str">
-        <v xml:space="preserve">                   ne</v>
-      </c>
-      <c r="I49" t="str">
+      <c r="F49" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G49" t="str">
         <v xml:space="preserve">                   ne</v>
       </c>
     </row>
@@ -1794,16 +1548,10 @@
       <c r="E50">
         <v>0</v>
       </c>
-      <c r="F50">
-        <v>0</v>
-      </c>
-      <c r="G50">
-        <v>0</v>
-      </c>
-      <c r="H50" t="str">
-        <v xml:space="preserve">                   ne</v>
-      </c>
-      <c r="I50" t="str">
+      <c r="F50" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G50" t="str">
         <v xml:space="preserve">                   ne</v>
       </c>
     </row>
@@ -1823,29 +1571,23 @@
       <c r="E51">
         <v>0</v>
       </c>
-      <c r="F51">
-        <v>0</v>
-      </c>
-      <c r="G51">
-        <v>0</v>
-      </c>
-      <c r="H51" t="str">
-        <v xml:space="preserve">                   ne</v>
-      </c>
-      <c r="I51" t="str">
+      <c r="F51" t="str">
+        <v xml:space="preserve">                   ne</v>
+      </c>
+      <c r="G51" t="str">
         <v xml:space="preserve">                   ne</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I51"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G51"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1860,39 +1602,23 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Auf 1</v>
+        <v>dfe</v>
       </c>
       <c r="B2">
-        <v>9</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Auf 2</v>
+        <v>ewwr</v>
       </c>
       <c r="B3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Auf 3</v>
-      </c>
-      <c r="B4">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Auf 4</v>
-      </c>
-      <c r="B5">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B3"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -2022,7 +1748,7 @@
         <v>Exportdatum</v>
       </c>
       <c r="B6" t="str">
-        <v>24.2.2025</v>
+        <v>4.3.2025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>